<commit_message>
added download history of leases
</commit_message>
<xml_diff>
--- a/data/exel-docs/barcha-ijaralar.xlsx
+++ b/data/exel-docs/barcha-ijaralar.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -422,92 +422,71 @@
         <v>studentPhoneNumber</v>
       </c>
       <c r="G1" t="str">
-        <v>active</v>
+        <v>orderedTime</v>
       </c>
       <c r="H1" t="str">
-        <v>orderedTime</v>
-      </c>
-      <c r="I1" t="str">
         <v>deadline</v>
-      </c>
-      <c r="J1" t="str">
-        <v>slug</v>
-      </c>
-      <c r="K1" t="str">
-        <v>shouldBeReturned</v>
-      </c>
-      <c r="L1" t="str">
-        <v>id</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Jo'rayev Narimon</v>
+        <v>Bakhodirova  Rukhsorakhon  Behzod qizi</v>
+      </c>
+      <c r="B2" t="str">
+        <v>6389c809666ce69a7f92ffa9</v>
       </c>
       <c r="C2" t="str">
-        <v>CH-00092</v>
+        <v>CH-00118</v>
       </c>
       <c r="D2" t="str">
-        <v>E202</v>
+        <v>E-203</v>
       </c>
       <c r="E2" t="str">
         <v>ECE</v>
       </c>
       <c r="F2" t="str">
-        <v>+998911234567</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
+        <v xml:space="preserve"> 998 97 4633882</v>
+      </c>
+      <c r="G2" t="str">
+        <v>2022-12-10T09:36:53.998Z</v>
       </c>
       <c r="H2" t="str">
-        <v>2022-12-06T11:19:56.130Z</v>
-      </c>
-      <c r="I2" t="str">
-        <v>2022-12-13T11:19:56.130Z</v>
-      </c>
-      <c r="J2" t="str">
-        <v>jo'rayev-narimon-ece-e202</v>
-      </c>
-      <c r="K2" t="b">
-        <v>0</v>
+        <v>2022-12-17T09:36:53.998Z</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Mahmudhodjayev Izzat</v>
+        <v>Tulaev  Muhammad  Dilshod o‘g‘li</v>
+      </c>
+      <c r="B3" t="str">
+        <v>638f8d2f008bc82d3ca29407</v>
       </c>
       <c r="C3" t="str">
-        <v>CH-00017</v>
+        <v>N-01597</v>
       </c>
       <c r="D3" t="str">
-        <v>A203</v>
+        <v>E-203</v>
       </c>
       <c r="E3" t="str">
-        <v>Architecture</v>
+        <v>ECE</v>
       </c>
       <c r="F3" t="str">
-        <v>+998977654321</v>
-      </c>
-      <c r="G3" t="b">
-        <v>1</v>
+        <v xml:space="preserve"> 998 90 864-20-24</v>
+      </c>
+      <c r="G3" t="str">
+        <v>2022-12-10T09:33:35.871Z</v>
       </c>
       <c r="H3" t="str">
-        <v>2022-12-06T11:35:38.491Z</v>
-      </c>
-      <c r="I3" t="str">
-        <v>2022-12-13T11:35:38.491Z</v>
-      </c>
-      <c r="J3" t="str">
-        <v>mahmudhodjayev-izzat-architecture-a203</v>
-      </c>
-      <c r="K3" t="b">
-        <v>0</v>
+        <v>2022-12-17T09:33:35.871Z</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
         <v>Umedov Dilshod</v>
       </c>
+      <c r="B4" t="str">
+        <v>638f8cb7008bc82d3ca29401</v>
+      </c>
       <c r="C4" t="str">
         <v>N-01590</v>
       </c>
@@ -520,60 +499,48 @@
       <c r="F4" t="str">
         <v>+99891312212</v>
       </c>
-      <c r="G4" t="b">
-        <v>1</v>
+      <c r="G4" t="str">
+        <v>2022-12-06T21:03:48.510Z</v>
       </c>
       <c r="H4" t="str">
-        <v>2022-12-06T21:03:48.510Z</v>
-      </c>
-      <c r="I4" t="str">
         <v>2022-12-13T21:03:48.510Z</v>
-      </c>
-      <c r="J4" t="str">
-        <v>umedov-dilshod-ece-e202</v>
-      </c>
-      <c r="K4" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Adizov No'mon</v>
+        <v>Mahmudhodjayev Izzat</v>
+      </c>
+      <c r="B5" t="str">
+        <v>6389c809666ce69a7f92ffaa</v>
       </c>
       <c r="C5" t="str">
-        <v>CH-00093</v>
+        <v>CH-00017</v>
       </c>
       <c r="D5" t="str">
-        <v>E201</v>
+        <v>A203</v>
       </c>
       <c r="E5" t="str">
-        <v>ECE</v>
+        <v>Architecture</v>
       </c>
       <c r="F5" t="str">
-        <v>+998900011112</v>
-      </c>
-      <c r="G5" t="b">
-        <v>1</v>
+        <v>+998977654321</v>
+      </c>
+      <c r="G5" t="str">
+        <v>2022-12-06T11:35:38.491Z</v>
       </c>
       <c r="H5" t="str">
-        <v>2022-12-07T06:52:04.466Z</v>
-      </c>
-      <c r="I5" t="str">
-        <v>2022-12-14T06:52:04.466Z</v>
-      </c>
-      <c r="J5" t="str">
-        <v>adizov-no'mon-ece-e201</v>
-      </c>
-      <c r="K5" t="b">
-        <v>0</v>
+        <v>2022-12-13T11:35:38.491Z</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Sodiqov Otabek</v>
+        <v>Jo'rayev Narimon</v>
+      </c>
+      <c r="B6" t="str">
+        <v>6389c809666ce69a7f92ffac</v>
       </c>
       <c r="C6" t="str">
-        <v>CH-00020</v>
+        <v>CH-00092</v>
       </c>
       <c r="D6" t="str">
         <v>E202</v>
@@ -582,59 +549,18 @@
         <v>ECE</v>
       </c>
       <c r="F6" t="str">
-        <v>+998900234321</v>
-      </c>
-      <c r="G6" t="b">
-        <v>1</v>
+        <v>+998911234567</v>
+      </c>
+      <c r="G6" t="str">
+        <v>2022-12-06T11:19:56.130Z</v>
       </c>
       <c r="H6" t="str">
-        <v>2022-12-07T06:58:11.530Z</v>
-      </c>
-      <c r="I6" t="str">
-        <v>2022-12-14T06:58:11.530Z</v>
-      </c>
-      <c r="J6" t="str">
-        <v>sodiqov-otabek-ece-e202</v>
-      </c>
-      <c r="K6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Sodiqov Otabek</v>
-      </c>
-      <c r="C7" t="str">
-        <v>CH-00021</v>
-      </c>
-      <c r="D7" t="str">
-        <v>E202</v>
-      </c>
-      <c r="E7" t="str">
-        <v>ECE</v>
-      </c>
-      <c r="F7" t="str">
-        <v>+998900010101</v>
-      </c>
-      <c r="G7" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" t="str">
-        <v>2022-12-07T06:59:14.163Z</v>
-      </c>
-      <c r="I7" t="str">
-        <v>2022-12-14T06:59:14.163Z</v>
-      </c>
-      <c r="J7" t="str">
-        <v>sodiqov-otabek-ece-e202</v>
-      </c>
-      <c r="K7" t="b">
-        <v>0</v>
+        <v>2022-12-13T11:19:56.130Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>